<commit_message>
- Fix iteration - Update test excel
</commit_message>
<xml_diff>
--- a/tests/data/Individuals.xlsx
+++ b/tests/data/Individuals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub repositories\ESQlabs\esqlabsR\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B892C6-F7F8-435F-9A5D-35CB5308BD4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A305424-E982-478F-A648-EB087D54F046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IndividualBiometrics" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Human</t>
   </si>
@@ -75,10 +75,7 @@
     <t>Individual_with_NAs</t>
   </si>
   <si>
-    <t>Protein</t>
-  </si>
-  <si>
-    <t>Ontogeny</t>
+    <t>Protein Ontogenies</t>
   </si>
 </sst>
 </file>
@@ -402,31 +399,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.41015625" customWidth="1"/>
-    <col min="2" max="2" width="6.87890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.29296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.41015625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.41015625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.1171875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="8.41015625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.41015625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -451,11 +448,8 @@
       <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -478,7 +472,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -501,7 +495,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -523,6 +517,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6960b7ce0e258e5d224c1a71edff679">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7db7ba54f101f424e932c64edcbdaa0" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -739,15 +742,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -755,6 +749,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78CA0B51-7456-4883-901E-100C95177B36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EEA776C-4DAB-4C30-9CC1-14DE8CBA854F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -773,14 +775,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78CA0B51-7456-4883-901E-100C95177B36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028903B1-0B22-4BE6-8A73-043144867A27}">
   <ds:schemaRefs>

</xml_diff>